<commit_message>
added deck addition and deck update logs
</commit_message>
<xml_diff>
--- a/custom_statuses.xlsx
+++ b/custom_statuses.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B284"/>
+  <dimension ref="A1:B290"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2678,9 +2678,57 @@
         <v>depressedmonke</v>
       </c>
     </row>
+    <row r="285">
+      <c r="A285" t="str">
+        <v>Attempting to softlock irl by biting a cactus</v>
+      </c>
+      <c r="B285" t="str">
+        <v>depressedmonke_</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="str">
+        <v>Mono gang</v>
+      </c>
+      <c r="B286" t="str">
+        <v>waltuh</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="str">
+        <v>Playing Celestial Custodian in Graveyard to correct its turn order</v>
+      </c>
+      <c r="B287" t="str">
+        <v>depressedmonke_</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="str">
+        <v>Ten likes and Huyn draws Swabbie with huge muscles and abs</v>
+      </c>
+      <c r="B288" t="str">
+        <v>lumpymilktea</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="str">
+        <v>Taking deckbuilding lessons from Crimpton 🛹</v>
+      </c>
+      <c r="B289" t="str">
+        <v>depressedmonke_</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="str">
+        <v>Ferb, I know what we're gonna do today!</v>
+      </c>
+      <c r="B290" t="str">
+        <v>Tbone</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B284"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B290"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved tbot to slash commands
</commit_message>
<xml_diff>
--- a/custom_statuses.xlsx
+++ b/custom_statuses.xlsx
@@ -397,13 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B290"/>
+  <dimension ref="A1:B298"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="100.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2726,9 +2726,73 @@
         <v>Tbone</v>
       </c>
     </row>
+    <row r="291">
+      <c r="A291" t="str">
+        <v>Spinning the wheel for which widely-considered-mediocre card is now busted because of a certain tech</v>
+      </c>
+      <c r="B291" t="str">
+        <v>stingray</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="str">
+        <v>Getting mass downvoted after explaining why ANB isn't S tier</v>
+      </c>
+      <c r="B292" t="str">
+        <v>4-Pound Plate of Pasta</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="str">
+        <v>Gee i sure hope I don't miss this eyespore fusion</v>
+      </c>
+      <c r="B293" t="str">
+        <v>4-Pound Plate of Pasta</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="str">
+        <v>Reading the 400th crippling DMD nerf on the sub</v>
+      </c>
+      <c r="B294" t="str">
+        <v>4-Pound Plate of Pasta</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="str">
+        <v>Roping my opponent so I can listen to the low health theme</v>
+      </c>
+      <c r="B295" t="str">
+        <v>4-Pound Plate of Pasta</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="str">
+        <v>Running Buff-Shroom in Cycle-Cap to counter ZM Sig</v>
+      </c>
+      <c r="B296" t="str">
+        <v>4-Pound Plate of Pasta</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="str">
+        <v>Getting a Magic Beanstalk from the 15 daily streak reward</v>
+      </c>
+      <c r="B297" t="str">
+        <v>4-Pound Plate of Pasta</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="str">
+        <v>getting nothing because it's not worth logging in</v>
+      </c>
+      <c r="B298" t="str">
+        <v>Stingray</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B290"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B298"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating a couple files
</commit_message>
<xml_diff>
--- a/custom_statuses.xlsx
+++ b/custom_statuses.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B298"/>
+  <dimension ref="A1:B308"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2790,9 +2790,89 @@
         <v>Stingray</v>
       </c>
     </row>
+    <row r="299">
+      <c r="A299" t="str">
+        <v>Using Eyespore as an aggro card</v>
+      </c>
+      <c r="B299" t="str">
+        <v>Durga</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="str">
+        <v>Ign: 40anb swr</v>
+      </c>
+      <c r="B300" t="str">
+        <v>Durga</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="str">
+        <v>Sunshroom is destroying the meta, nerf Miner</v>
+      </c>
+      <c r="B301" t="str">
+        <v>FrozenFighter</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="str">
+        <v>With Reincarnation, VRH and Fig, we could be able to get a Reliable Molekale..... stares at camera</v>
+      </c>
+      <c r="B302" t="str">
+        <v>StingRay</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="str">
+        <v>When your Molekale spawns a Pineclone</v>
+      </c>
+      <c r="B303" t="str">
+        <v>Frozen Fighter</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="str">
+        <v>turn 1 black hole turn 2 double cheese</v>
+      </c>
+      <c r="B304" t="str">
+        <v>Huyn</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="str">
+        <v>rose is so OP why won't my 4x5 HG conjure pile work on her???</v>
+      </c>
+      <c r="B305" t="str">
+        <v>StingRay</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="str">
+        <v>Fighting for Corndog</v>
+      </c>
+      <c r="B306" t="str">
+        <v>Waltuh</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="str">
+        <v>Which hero can play OTK Cryo Yeti? HG? No. BF? No. GS? Yes.</v>
+      </c>
+      <c r="B307" t="str">
+        <v>connorthepeach</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="str">
+        <v>Helping Vengeful Cyborg look for his lost toupee</v>
+      </c>
+      <c r="B308" t="str">
+        <v>Pasta</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B298"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B308"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>